<commit_message>
CAS plan import/export files completed
</commit_message>
<xml_diff>
--- a/04_BugAndEnhancementList.xlsx
+++ b/04_BugAndEnhancementList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PietervanZyl\Documents\GitHub\CMMITools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E59301D-FD3D-48DD-8716-8F8888554076}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2280E0-A713-4A53-BFB9-091538D3B4FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Remove. Not used</t>
+  </si>
+  <si>
+    <t>HIGH IMPORTANCE: Put a message that people make sure processess has been listed correctly before the OEdb is generated.</t>
+  </si>
+  <si>
+    <t>Prioritised</t>
   </si>
 </sst>
 </file>
@@ -426,17 +432,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="8.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38.08984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="43.36328125" style="1" customWidth="1"/>
     <col min="6" max="6" width="55.1796875" style="1" customWidth="1"/>
     <col min="7" max="7" width="49.81640625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="17.6328125" style="1"/>
@@ -571,6 +577,23 @@
         <v>22</v>
       </c>
     </row>
+    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>44226</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>